<commit_message>
doc(jnltrav): update pour 27.09
</commit_message>
<xml_diff>
--- a/Documentation/Journal-de-Travail_KhalilMateen.xlsx
+++ b/Documentation/Journal-de-Travail_KhalilMateen.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pq40rdc\Documents\GitHub\P_FUN_matkha\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BF2BA93-7794-403E-BD67-29686D7BD8F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A146B63-4DFC-4EBB-803A-964563544CBA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="Mvap2W10CJFFJsnvkGXSiMLvpngxTMJbJsIKFe7Hzjn0XDcmjGuvBC2FjUCZ/hpRpUhUrG1T4kBlDAIo3yqmSQ==" workbookSaltValue="KXjgXOcsUZI/j7UgPKltzw==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
     <workbookView xWindow="3630" yWindow="1875" windowWidth="21600" windowHeight="11385" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="46">
   <si>
     <t>Journal de travail</t>
   </si>
@@ -173,6 +173,12 @@
   </si>
   <si>
     <t xml:space="preserve">j'ai essayé plusieur api (officiel et non officiels) pour importer les data que j'avais besoin pour afficher le nombre de joueur en ligne mais aucune ne marchais/me donnais les info dont j'avais besoin, j'ai trouvé un outils (steamkit) qui me permet apparement de faire ce dont j'ai besoin mais malheuresmenet il a très peu de documentation </t>
+  </si>
+  <si>
+    <t>j'ai réussi a faire en sorte que quand mon app se lance elle prends les data du .json elle organise et les affiche dans le graphique oxyplot</t>
+  </si>
+  <si>
+    <t>j'ai fait en sorte que quand on change le type de filtrage du temps, elle change les données qu'elle prends du json -&gt; si on change de heure a jour elle prends les données du jour</t>
   </si>
 </sst>
 </file>
@@ -476,6 +482,9 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="16" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
       <protection locked="0"/>
@@ -483,162 +492,11 @@
     <xf numFmtId="20" fontId="5" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="25">
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF0070C0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF7030A0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1" tint="0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFCCCC00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF0070C0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF7030A0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1" tint="0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFCCCC00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -807,6 +665,154 @@
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
           <bgColor theme="2" tint="-9.9978637043366805E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF0070C0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="2" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF7030A0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="1" tint="0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFCCCC00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF0070C0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="2" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF7030A0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="1" tint="0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFCCCC00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="-0.24994659260841701"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1170,7 +1176,7 @@
                   <c:v>4.8611111111111112E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.22222222222222221</c:v>
+                  <c:v>0.3298611111111111</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
@@ -1894,18 +1900,18 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{F2213DF1-F6B1-174C-AC17-4E96BE96C00D}" name="Table1" displayName="Table1" ref="A6:G532" totalsRowShown="0" headerRowDxfId="24" tableBorderDxfId="23">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{F2213DF1-F6B1-174C-AC17-4E96BE96C00D}" name="Table1" displayName="Table1" ref="A6:G532" totalsRowShown="0" headerRowDxfId="8" tableBorderDxfId="7">
   <autoFilter ref="A6:G532" xr:uid="{F2213DF1-F6B1-174C-AC17-4E96BE96C00D}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{315BA4B4-9BD9-AB4E-8D40-FABFA0BB2AEA}" name="Semaine" dataDxfId="22">
+    <tableColumn id="1" xr3:uid="{315BA4B4-9BD9-AB4E-8D40-FABFA0BB2AEA}" name="Semaine" dataDxfId="6">
       <calculatedColumnFormula>IF(ISBLANK(B7),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B7))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{503C31E9-854D-BF42-85AC-8DFA1376C4D8}" name="Jour" dataDxfId="21"/>
-    <tableColumn id="3" xr3:uid="{B35A0B98-71A0-BA4F-BFAB-00A05EA1F23A}" name="heure" dataDxfId="20"/>
-    <tableColumn id="4" xr3:uid="{BE4D837D-FC99-BA48-A82F-B8C8E4CE5BF8}" name="min." dataDxfId="19"/>
-    <tableColumn id="5" xr3:uid="{A2DCC539-6D2A-B04A-BF8E-6FACE6268D1F}" name="Activité" dataDxfId="18"/>
-    <tableColumn id="6" xr3:uid="{4EA406B9-7EF7-D547-AF98-5AD11BE168E9}" name="Description" dataDxfId="17"/>
-    <tableColumn id="7" xr3:uid="{1735360B-2647-6D42-A0E3-3425EE302FFD}" name="Remarque / problème" dataDxfId="16"/>
+    <tableColumn id="2" xr3:uid="{503C31E9-854D-BF42-85AC-8DFA1376C4D8}" name="Jour" dataDxfId="5"/>
+    <tableColumn id="3" xr3:uid="{B35A0B98-71A0-BA4F-BFAB-00A05EA1F23A}" name="heure" dataDxfId="4"/>
+    <tableColumn id="4" xr3:uid="{BE4D837D-FC99-BA48-A82F-B8C8E4CE5BF8}" name="min." dataDxfId="3"/>
+    <tableColumn id="5" xr3:uid="{A2DCC539-6D2A-B04A-BF8E-6FACE6268D1F}" name="Activité" dataDxfId="2"/>
+    <tableColumn id="6" xr3:uid="{4EA406B9-7EF7-D547-AF98-5AD11BE168E9}" name="Description" dataDxfId="1"/>
+    <tableColumn id="7" xr3:uid="{1735360B-2647-6D42-A0E3-3425EE302FFD}" name="Remarque / problème" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2100,8 +2106,8 @@
   <dimension ref="A1:O532"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="6" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E24" sqref="E24"/>
+      <pane ySplit="6" topLeftCell="A19" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2136,11 +2142,11 @@
       <c r="B2" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="55" t="s">
+      <c r="C2" s="56" t="s">
         <v>29</v>
       </c>
-      <c r="D2" s="55"/>
-      <c r="E2" s="55"/>
+      <c r="D2" s="56"/>
+      <c r="E2" s="56"/>
       <c r="F2" s="5" t="s">
         <v>2</v>
       </c>
@@ -2154,7 +2160,7 @@
       </c>
       <c r="C3" s="23" t="str">
         <f>INT(E4/1440)&amp;" jours "&amp;INT(MOD(E4/1440,1)*24)&amp;" heurs "&amp;INT(MOD(MOD(E4/1440,1)*24,1)*60)&amp;" minutes"</f>
-        <v>0 jours 12 heurs 9 minutes</v>
+        <v>0 jours 14 heurs 45 minutes</v>
       </c>
       <c r="D3" s="23"/>
       <c r="E3" s="3"/>
@@ -2169,24 +2175,24 @@
       <c r="B4" s="5"/>
       <c r="C4" s="23">
         <f>SUBTOTAL(9,$C$7:$C$531)*60</f>
-        <v>420</v>
+        <v>540</v>
       </c>
       <c r="D4" s="23">
         <f>SUBTOTAL(9,$D$7:$D$531)</f>
-        <v>310</v>
+        <v>345</v>
       </c>
       <c r="E4" s="41">
         <f>SUM(C4:D4)</f>
-        <v>730</v>
+        <v>885</v>
       </c>
       <c r="F4" s="4"/>
       <c r="G4" s="7"/>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="C5" s="56" t="s">
+      <c r="C5" s="57" t="s">
         <v>16</v>
       </c>
-      <c r="D5" s="56"/>
+      <c r="D5" s="57"/>
     </row>
     <row r="6" spans="1:15" s="21" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="19" t="s">
@@ -2569,7 +2575,7 @@
       <c r="B21" s="51"/>
       <c r="C21" s="52"/>
       <c r="D21" s="53"/>
-      <c r="E21" s="57"/>
+      <c r="E21" s="55"/>
       <c r="F21" s="54"/>
       <c r="G21" s="18"/>
     </row>
@@ -2593,28 +2599,44 @@
       </c>
       <c r="G22" s="16"/>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A23" s="17" t="str">
+    <row r="23" spans="1:15" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A23" s="17">
         <f>IF(ISBLANK(B23),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B23))</f>
-        <v/>
-      </c>
-      <c r="B23" s="51"/>
-      <c r="C23" s="52"/>
-      <c r="D23" s="53"/>
-      <c r="E23" s="54"/>
-      <c r="F23" s="37"/>
+        <v>39</v>
+      </c>
+      <c r="B23" s="51">
+        <v>45562</v>
+      </c>
+      <c r="C23" s="52">
+        <v>2</v>
+      </c>
+      <c r="D23" s="53">
+        <v>0</v>
+      </c>
+      <c r="E23" s="54" t="s">
+        <v>4</v>
+      </c>
+      <c r="F23" s="37" t="s">
+        <v>44</v>
+      </c>
       <c r="G23" s="18"/>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:15" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A24" s="8" t="str">
         <f>IF(ISBLANK(B24),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B24))</f>
         <v/>
       </c>
       <c r="B24" s="47"/>
       <c r="C24" s="48"/>
-      <c r="D24" s="49"/>
-      <c r="E24" s="50"/>
-      <c r="F24" s="37"/>
+      <c r="D24" s="49">
+        <v>35</v>
+      </c>
+      <c r="E24" s="50" t="s">
+        <v>4</v>
+      </c>
+      <c r="F24" s="37" t="s">
+        <v>45</v>
+      </c>
       <c r="G24" s="16"/>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.25">
@@ -8720,54 +8742,54 @@
     <mergeCell ref="C5:D5"/>
   </mergeCells>
   <conditionalFormatting sqref="E7:E20 E22:E532">
-    <cfRule type="expression" dxfId="15" priority="1">
+    <cfRule type="expression" dxfId="24" priority="1">
       <formula>$E7="Autre"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="14" priority="2" stopIfTrue="1">
+    <cfRule type="expression" dxfId="23" priority="2" stopIfTrue="1">
       <formula>$E7="Design"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="13" priority="3" stopIfTrue="1">
+    <cfRule type="expression" dxfId="22" priority="3" stopIfTrue="1">
       <formula>$E7="Présentation"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="12" priority="4" stopIfTrue="1">
+    <cfRule type="expression" dxfId="21" priority="4" stopIfTrue="1">
       <formula>$E7="Meeting"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="11" priority="5" stopIfTrue="1">
+    <cfRule type="expression" dxfId="20" priority="5" stopIfTrue="1">
       <formula>$E7="Documentation"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="10" priority="6" stopIfTrue="1">
+    <cfRule type="expression" dxfId="19" priority="6" stopIfTrue="1">
       <formula>$E7="Test"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="9" priority="7" stopIfTrue="1">
+    <cfRule type="expression" dxfId="18" priority="7" stopIfTrue="1">
       <formula>$E7="Analyse"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="8" priority="9" stopIfTrue="1">
+    <cfRule type="expression" dxfId="17" priority="9" stopIfTrue="1">
       <formula>$E7="Développement"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F21">
-    <cfRule type="expression" dxfId="7" priority="18">
+    <cfRule type="expression" dxfId="16" priority="18">
       <formula>$F21="Autre"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="6" priority="19" stopIfTrue="1">
+    <cfRule type="expression" dxfId="15" priority="19" stopIfTrue="1">
       <formula>$F21="Design"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="5" priority="20" stopIfTrue="1">
+    <cfRule type="expression" dxfId="14" priority="20" stopIfTrue="1">
       <formula>$F21="Présentation"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="4" priority="21" stopIfTrue="1">
+    <cfRule type="expression" dxfId="13" priority="21" stopIfTrue="1">
       <formula>$F21="Meeting"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="3" priority="22" stopIfTrue="1">
+    <cfRule type="expression" dxfId="12" priority="22" stopIfTrue="1">
       <formula>$F21="Documentation"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="2" priority="23" stopIfTrue="1">
+    <cfRule type="expression" dxfId="11" priority="23" stopIfTrue="1">
       <formula>$F21="Test"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="1" priority="24" stopIfTrue="1">
+    <cfRule type="expression" dxfId="10" priority="24" stopIfTrue="1">
       <formula>$F21="Analyse"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="0" priority="25" stopIfTrue="1">
+    <cfRule type="expression" dxfId="9" priority="25" stopIfTrue="1">
       <formula>$F21="Développement"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -8842,11 +8864,11 @@
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Analyse!C5,'Journal de travail'!$C$7:$C$532)*60</f>
-        <v>300</v>
+        <v>420</v>
       </c>
       <c r="B5">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Analyse!C5,'Journal de travail'!$D$7:$D$532)</f>
-        <v>20</v>
+        <v>55</v>
       </c>
       <c r="C5" s="42" t="str">
         <f>'Journal de travail'!M9</f>
@@ -8854,7 +8876,7 @@
       </c>
       <c r="D5" s="34">
         <f t="shared" ref="D5:D11" si="0">(A5+B5)/1440</f>
-        <v>0.22222222222222221</v>
+        <v>0.3298611111111111</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
@@ -8963,7 +8985,7 @@
       </c>
       <c r="D12" s="35">
         <f>SUM(D4:D11)</f>
-        <v>0.46527777777777773</v>
+        <v>0.57291666666666674</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
@@ -8986,17 +9008,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="be0d3259-a7ce-4623-88ec-81594dfcbc1c" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="99ffe1f3-7857-457f-add0-5bdef636f38d">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100D4F20F00DBE2EE49BE9523363A2DF18B" ma:contentTypeVersion="13" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="313dbdbec26224d1c2bb7e3c488b2a4e">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="99ffe1f3-7857-457f-add0-5bdef636f38d" xmlns:ns3="be0d3259-a7ce-4623-88ec-81594dfcbc1c" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4739345e3d2c6be79c5ae1a54d02a4a7" ns2:_="" ns3:_="">
     <xsd:import namespace="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
@@ -9219,6 +9230,17 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="be0d3259-a7ce-4623-88ec-81594dfcbc1c" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="99ffe1f3-7857-457f-add0-5bdef636f38d">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74326215-CB02-4E95-BFFB-9EC625B1BF0F}">
   <ds:schemaRefs>
@@ -9228,17 +9250,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0453EC0E-0298-408B-815C-A1500DB4F5E9}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="be0d3259-a7ce-4623-88ec-81594dfcbc1c"/>
-    <ds:schemaRef ds:uri="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F2FB702A-DCBD-43A8-A34C-6000FD8861AD}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -9255,4 +9266,15 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0453EC0E-0298-408B-815C-A1500DB4F5E9}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="be0d3259-a7ce-4623-88ec-81594dfcbc1c"/>
+    <ds:schemaRef ds:uri="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
chore(jntlrav): mise ajour journal de travail 11.10
</commit_message>
<xml_diff>
--- a/Documentation/Journal-de-Travail_KhalilMateen.xlsx
+++ b/Documentation/Journal-de-Travail_KhalilMateen.xlsx
@@ -8,10 +8,10 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pq40rdc\Documents\GitHub\P_FUN_matkha\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A146B63-4DFC-4EBB-803A-964563544CBA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83FA3969-DB6E-48E1-B597-0FB84FCB437E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="Mvap2W10CJFFJsnvkGXSiMLvpngxTMJbJsIKFe7Hzjn0XDcmjGuvBC2FjUCZ/hpRpUhUrG1T4kBlDAIo3yqmSQ==" workbookSaltValue="KXjgXOcsUZI/j7UgPKltzw==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
-    <workbookView xWindow="3630" yWindow="1875" windowWidth="21600" windowHeight="11385" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
   </bookViews>
   <sheets>
     <sheet name="Journal de travail" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="53">
   <si>
     <t>Journal de travail</t>
   </si>
@@ -179,6 +179,27 @@
   </si>
   <si>
     <t>j'ai fait en sorte que quand on change le type de filtrage du temps, elle change les données qu'elle prends du json -&gt; si on change de heure a jour elle prends les données du jour</t>
+  </si>
+  <si>
+    <t xml:space="preserve">abcence </t>
+  </si>
+  <si>
+    <t>refactorisation des méthodes dans la classe region data pour mettre en place linq</t>
+  </si>
+  <si>
+    <t>le prof nous a expliquer des attentes par rapport au projet</t>
+  </si>
+  <si>
+    <t>le prof nous a montrer les outils "plantuml" et "icetools"</t>
+  </si>
+  <si>
+    <t>mise en place de icetools (token de icescrum et configuration du fichier .js)</t>
+  </si>
+  <si>
+    <t>j'ai fais un schémas pour la user story "Manière d'afficher les nombres de joueurs steam"</t>
+  </si>
+  <si>
+    <t>rédiger user story, et les faire corriger par le porf, il ma donné un feed back</t>
   </si>
 </sst>
 </file>
@@ -1176,16 +1197,16 @@
                   <c:v>4.8611111111111112E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.3298611111111111</c:v>
+                  <c:v>0.34722222222222221</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>8.6805555555555552E-2</c:v>
+                  <c:v>0.1701388888888889</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>2.4305555555555556E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>7.6388888888888895E-2</c:v>
@@ -2106,8 +2127,8 @@
   <dimension ref="A1:O532"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="6" topLeftCell="A19" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F24" sqref="F24"/>
+      <pane ySplit="6" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F32" sqref="F32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2160,7 +2181,7 @@
       </c>
       <c r="C3" s="23" t="str">
         <f>INT(E4/1440)&amp;" jours "&amp;INT(MOD(E4/1440,1)*24)&amp;" heurs "&amp;INT(MOD(MOD(E4/1440,1)*24,1)*60)&amp;" minutes"</f>
-        <v>0 jours 14 heurs 45 minutes</v>
+        <v>0 jours 20 heurs 45 minutes</v>
       </c>
       <c r="D3" s="23"/>
       <c r="E3" s="3"/>
@@ -2175,15 +2196,15 @@
       <c r="B4" s="5"/>
       <c r="C4" s="23">
         <f>SUBTOTAL(9,$C$7:$C$531)*60</f>
-        <v>540</v>
+        <v>780</v>
       </c>
       <c r="D4" s="23">
         <f>SUBTOTAL(9,$D$7:$D$531)</f>
-        <v>345</v>
+        <v>465</v>
       </c>
       <c r="E4" s="41">
         <f>SUM(C4:D4)</f>
-        <v>885</v>
+        <v>1245</v>
       </c>
       <c r="F4" s="4"/>
       <c r="G4" s="7"/>
@@ -2640,27 +2661,43 @@
       <c r="G24" s="16"/>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A25" s="17" t="str">
+      <c r="A25" s="17">
         <f>IF(ISBLANK(B25),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B25))</f>
-        <v/>
-      </c>
-      <c r="B25" s="51"/>
-      <c r="C25" s="52"/>
+        <v>36</v>
+      </c>
+      <c r="B25" s="51">
+        <v>45540</v>
+      </c>
+      <c r="C25" s="52">
+        <v>3</v>
+      </c>
       <c r="D25" s="53"/>
-      <c r="E25" s="54"/>
-      <c r="F25" s="37"/>
+      <c r="E25" s="54" t="s">
+        <v>22</v>
+      </c>
+      <c r="F25" s="37" t="s">
+        <v>46</v>
+      </c>
       <c r="G25" s="18"/>
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A26" s="8" t="str">
+      <c r="A26" s="8">
         <f>IF(ISBLANK(B26),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B26))</f>
-        <v/>
-      </c>
-      <c r="B26" s="47"/>
+        <v>41</v>
+      </c>
+      <c r="B26" s="47">
+        <v>45576</v>
+      </c>
       <c r="C26" s="48"/>
-      <c r="D26" s="49"/>
-      <c r="E26" s="50"/>
-      <c r="F26" s="37"/>
+      <c r="D26" s="49">
+        <v>25</v>
+      </c>
+      <c r="E26" s="50" t="s">
+        <v>4</v>
+      </c>
+      <c r="F26" s="37" t="s">
+        <v>47</v>
+      </c>
       <c r="G26" s="16"/>
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.25">
@@ -2670,9 +2707,15 @@
       </c>
       <c r="B27" s="51"/>
       <c r="C27" s="52"/>
-      <c r="D27" s="53"/>
-      <c r="E27" s="54"/>
-      <c r="F27" s="37"/>
+      <c r="D27" s="53">
+        <v>20</v>
+      </c>
+      <c r="E27" s="54" t="s">
+        <v>7</v>
+      </c>
+      <c r="F27" s="37" t="s">
+        <v>48</v>
+      </c>
       <c r="G27" s="18"/>
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.25">
@@ -2682,9 +2725,15 @@
       </c>
       <c r="B28" s="47"/>
       <c r="C28" s="48"/>
-      <c r="D28" s="49"/>
-      <c r="E28" s="50"/>
-      <c r="F28" s="36"/>
+      <c r="D28" s="49">
+        <v>15</v>
+      </c>
+      <c r="E28" s="50" t="s">
+        <v>7</v>
+      </c>
+      <c r="F28" s="36" t="s">
+        <v>49</v>
+      </c>
       <c r="G28" s="16"/>
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.25">
@@ -2694,9 +2743,15 @@
       </c>
       <c r="B29" s="51"/>
       <c r="C29" s="52"/>
-      <c r="D29" s="53"/>
-      <c r="E29" s="54"/>
-      <c r="F29" s="36"/>
+      <c r="D29" s="53">
+        <v>10</v>
+      </c>
+      <c r="E29" s="54" t="s">
+        <v>6</v>
+      </c>
+      <c r="F29" s="36" t="s">
+        <v>50</v>
+      </c>
       <c r="G29" s="18"/>
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.25">
@@ -2706,9 +2761,15 @@
       </c>
       <c r="B30" s="47"/>
       <c r="C30" s="48"/>
-      <c r="D30" s="49"/>
-      <c r="E30" s="50"/>
-      <c r="F30" s="37"/>
+      <c r="D30" s="49">
+        <v>5</v>
+      </c>
+      <c r="E30" s="50" t="s">
+        <v>6</v>
+      </c>
+      <c r="F30" s="37" t="s">
+        <v>51</v>
+      </c>
       <c r="G30" s="16"/>
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.25">
@@ -2717,10 +2778,18 @@
         <v/>
       </c>
       <c r="B31" s="51"/>
-      <c r="C31" s="52"/>
-      <c r="D31" s="53"/>
-      <c r="E31" s="54"/>
-      <c r="F31" s="36"/>
+      <c r="C31" s="52">
+        <v>1</v>
+      </c>
+      <c r="D31" s="53">
+        <v>45</v>
+      </c>
+      <c r="E31" s="54" t="s">
+        <v>6</v>
+      </c>
+      <c r="F31" s="36" t="s">
+        <v>52</v>
+      </c>
       <c r="G31" s="18"/>
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.25">
@@ -8868,7 +8937,7 @@
       </c>
       <c r="B5">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Analyse!C5,'Journal de travail'!$D$7:$D$532)</f>
-        <v>55</v>
+        <v>80</v>
       </c>
       <c r="C5" s="42" t="str">
         <f>'Journal de travail'!M9</f>
@@ -8876,7 +8945,7 @@
       </c>
       <c r="D5" s="34">
         <f t="shared" ref="D5:D11" si="0">(A5+B5)/1440</f>
-        <v>0.3298611111111111</v>
+        <v>0.34722222222222221</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
@@ -8900,11 +8969,11 @@
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Analyse!C7,'Journal de travail'!$C$7:$C$532)*60</f>
-        <v>0</v>
+        <v>60</v>
       </c>
       <c r="B7">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Analyse!C7,'Journal de travail'!$D$7:$D$532)</f>
-        <v>125</v>
+        <v>185</v>
       </c>
       <c r="C7" s="28" t="str">
         <f>'Journal de travail'!M11</f>
@@ -8912,7 +8981,7 @@
       </c>
       <c r="D7" s="34">
         <f t="shared" si="0"/>
-        <v>8.6805555555555552E-2</v>
+        <v>0.1701388888888889</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
@@ -8922,7 +8991,7 @@
       </c>
       <c r="B8">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Analyse!C8,'Journal de travail'!$D$7:$D$532)</f>
-        <v>0</v>
+        <v>35</v>
       </c>
       <c r="C8" s="29" t="str">
         <f>'Journal de travail'!M12</f>
@@ -8930,7 +8999,7 @@
       </c>
       <c r="D8" s="34">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2.4305555555555556E-2</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
@@ -8985,7 +9054,7 @@
       </c>
       <c r="D12" s="35">
         <f>SUM(D4:D11)</f>
-        <v>0.57291666666666674</v>
+        <v>0.69791666666666674</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
@@ -9008,6 +9077,17 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="be0d3259-a7ce-4623-88ec-81594dfcbc1c" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="99ffe1f3-7857-457f-add0-5bdef636f38d">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100D4F20F00DBE2EE49BE9523363A2DF18B" ma:contentTypeVersion="13" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="313dbdbec26224d1c2bb7e3c488b2a4e">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="99ffe1f3-7857-457f-add0-5bdef636f38d" xmlns:ns3="be0d3259-a7ce-4623-88ec-81594dfcbc1c" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4739345e3d2c6be79c5ae1a54d02a4a7" ns2:_="" ns3:_="">
     <xsd:import namespace="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
@@ -9230,17 +9310,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="be0d3259-a7ce-4623-88ec-81594dfcbc1c" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="99ffe1f3-7857-457f-add0-5bdef636f38d">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74326215-CB02-4E95-BFFB-9EC625B1BF0F}">
   <ds:schemaRefs>
@@ -9250,6 +9319,17 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0453EC0E-0298-408B-815C-A1500DB4F5E9}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="be0d3259-a7ce-4623-88ec-81594dfcbc1c"/>
+    <ds:schemaRef ds:uri="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F2FB702A-DCBD-43A8-A34C-6000FD8861AD}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -9266,15 +9346,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0453EC0E-0298-408B-815C-A1500DB4F5E9}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="be0d3259-a7ce-4623-88ec-81594dfcbc1c"/>
-    <ds:schemaRef ds:uri="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>